<commit_message>
emily chapter 1 edits
</commit_message>
<xml_diff>
--- a/book/data/demo.xlsx
+++ b/book/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44482</v>
+        <v>44483</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44481</v>
+        <v>44482</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44480</v>
+        <v>44481</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44479</v>
+        <v>44480</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44478</v>
+        <v>44479</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44477</v>
+        <v>44478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new chapters and lazy = FALSE
</commit_message>
<xml_diff>
--- a/book/data/demo.xlsx
+++ b/book/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44483</v>
+        <v>44484</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44482</v>
+        <v>44483</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44481</v>
+        <v>44482</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44480</v>
+        <v>44481</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44479</v>
+        <v>44480</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44478</v>
+        <v>44479</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
re-render with lisa edits to ch1 and 2
</commit_message>
<xml_diff>
--- a/book/data/demo.xlsx
+++ b/book/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44497</v>
+        <v>44507</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44496</v>
+        <v>44506</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44495</v>
+        <v>44505</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44494</v>
+        <v>44504</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44493</v>
+        <v>44503</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44492</v>
+        <v>44502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checked through ch 8
</commit_message>
<xml_diff>
--- a/book/data/demo.xlsx
+++ b/book/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44515</v>
+        <v>44522</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44514</v>
+        <v>44521</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44513</v>
+        <v>44520</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44512</v>
+        <v>44519</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44511</v>
+        <v>44518</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44510</v>
+        <v>44517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edits up through chapter 2
</commit_message>
<xml_diff>
--- a/book/data/demo.xlsx
+++ b/book/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44545</v>
+        <v>44564</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44544</v>
+        <v>44563</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44543</v>
+        <v>44562</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44542</v>
+        <v>44561</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44541</v>
+        <v>44560</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44540</v>
+        <v>44559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved summary chapter and made draft version
</commit_message>
<xml_diff>
--- a/book/data/demo.xlsx
+++ b/book/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44564</v>
+        <v>44566</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44563</v>
+        <v>44565</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44562</v>
+        <v>44564</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44561</v>
+        <v>44563</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44560</v>
+        <v>44562</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44559</v>
+        <v>44561</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Chapter 4 final edits
</commit_message>
<xml_diff>
--- a/book/data/demo.xlsx
+++ b/book/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44577</v>
+        <v>44578</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44576</v>
+        <v>44577</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44575</v>
+        <v>44576</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44574</v>
+        <v>44575</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44573</v>
+        <v>44574</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44572</v>
+        <v>44573</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
full render - including draft chapters
</commit_message>
<xml_diff>
--- a/book/data/demo.xlsx
+++ b/book/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44578</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44577</v>
+        <v>44579</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44576</v>
+        <v>44578</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44575</v>
+        <v>44577</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44574</v>
+        <v>44576</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44573</v>
+        <v>44575</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
verbatim and style changes
</commit_message>
<xml_diff>
--- a/book/data/demo.xlsx
+++ b/book/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44580</v>
+        <v>44581</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44579</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44578</v>
+        <v>44579</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44577</v>
+        <v>44578</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44576</v>
+        <v>44577</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44575</v>
+        <v>44576</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data types app edits
</commit_message>
<xml_diff>
--- a/book/data/demo.xlsx
+++ b/book/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44582</v>
+        <v>44585</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44581</v>
+        <v>44584</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44580</v>
+        <v>44583</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44579</v>
+        <v>44582</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44578</v>
+        <v>44581</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44577</v>
+        <v>44580</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
date extra info and spotify render
</commit_message>
<xml_diff>
--- a/book/data/demo.xlsx
+++ b/book/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44586</v>
+        <v>44588</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44585</v>
+        <v>44587</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44584</v>
+        <v>44586</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44583</v>
+        <v>44585</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44582</v>
+        <v>44584</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44581</v>
+        <v>44583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
various fixes and ch6 conflicting joins
</commit_message>
<xml_diff>
--- a/book/data/demo.xlsx
+++ b/book/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44588</v>
+        <v>44592</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44587</v>
+        <v>44591</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44586</v>
+        <v>44590</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44585</v>
+        <v>44589</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44584</v>
+        <v>44588</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44583</v>
+        <v>44587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ch2 clarification about library
</commit_message>
<xml_diff>
--- a/book/data/demo.xlsx
+++ b/book/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44595</v>
+        <v>44596</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44594</v>
+        <v>44595</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44593</v>
+        <v>44594</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44592</v>
+        <v>44593</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44591</v>
+        <v>44592</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44590</v>
+        <v>44591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
emily final chapter 8 edits
</commit_message>
<xml_diff>
--- a/book/data/demo.xlsx
+++ b/book/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44618</v>
+        <v>44619</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44617</v>
+        <v>44618</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44616</v>
+        <v>44617</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44615</v>
+        <v>44616</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44614</v>
+        <v>44615</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44613</v>
+        <v>44614</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ch 9 annotations section
</commit_message>
<xml_diff>
--- a/book/data/demo.xlsx
+++ b/book/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44619</v>
+        <v>44620</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44618</v>
+        <v>44619</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44617</v>
+        <v>44618</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44616</v>
+        <v>44617</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44615</v>
+        <v>44616</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44614</v>
+        <v>44615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
emily chapter 9 and 10 merge
</commit_message>
<xml_diff>
--- a/book/data/demo.xlsx
+++ b/book/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44620</v>
+        <v>44633</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44619</v>
+        <v>44632</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44618</v>
+        <v>44631</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44617</v>
+        <v>44630</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44616</v>
+        <v>44629</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44615</v>
+        <v>44628</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ch9 edits and full render
</commit_message>
<xml_diff>
--- a/book/data/demo.xlsx
+++ b/book/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44633</v>
+        <v>44634</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44632</v>
+        <v>44633</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44631</v>
+        <v>44632</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44630</v>
+        <v>44631</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44629</v>
+        <v>44630</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44628</v>
+        <v>44629</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final edits and rerender
</commit_message>
<xml_diff>
--- a/book/data/demo.xlsx
+++ b/book/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44636</v>
+        <v>44637</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44635</v>
+        <v>44636</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44634</v>
+        <v>44635</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44633</v>
+        <v>44634</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44632</v>
+        <v>44633</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44631</v>
+        <v>44632</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix typo in Ch 8
</commit_message>
<xml_diff>
--- a/book/data/demo.xlsx
+++ b/book/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44637</v>
+        <v>44648</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44636</v>
+        <v>44647</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44635</v>
+        <v>44646</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44634</v>
+        <v>44645</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44633</v>
+        <v>44644</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44632</v>
+        <v>44643</v>
       </c>
     </row>
   </sheetData>

</xml_diff>